<commit_message>
BMG gear to be 3mm
</commit_message>
<xml_diff>
--- a/files/HOTEND_EXTRUDER/DRAGON/BOM_HextrudORT_Extruder_Dragon.xlsx
+++ b/files/HOTEND_EXTRUDER/DRAGON/BOM_HextrudORT_Extruder_Dragon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\HOTEND_EXTRUDER\DRAGON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8425711-44F8-4977-A93A-3D0F4F622C3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D312B1B-C356-4A76-AB0D-2BD8E0574AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="81">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -92,23 +92,6 @@
   </si>
   <si>
     <t>Bondtech_Shaft_assembly v1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">From BMG Extruder
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*NOTE* Short side of the shaft might need to be filed down to avoid grinding against stepper motor.</t>
-    </r>
   </si>
   <si>
     <t>Bondtech_Thumbscrew_assembly v1</t>
@@ -370,12 +353,40 @@
   <si>
     <t>HARDWARE</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">From BMG Extruder
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*NOTE*
+1 - Some BMG clone have a 4mm thick gear, they will not fit.
+  Verified sources are: 
+  a) Original BMG from BondTech
+  b) https://s.click.aliexpress.com/e/_Ao9yaZ
+2 -  Short side of the shaft might need to be filed down to avoid grinding against stepper motor.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_Ao9yaZ</t>
+  </si>
+  <si>
+    <t>Triangle Lab</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,6 +492,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -604,10 +623,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -663,8 +683,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1995,24 +2019,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" customWidth="1"/>
+    <col min="5" max="5" width="37.54296875" customWidth="1"/>
+    <col min="6" max="6" width="23.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="9" max="9" width="76" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" customWidth="1"/>
-    <col min="11" max="11" width="42.140625" customWidth="1"/>
+    <col min="10" max="10" width="33.453125" customWidth="1"/>
+    <col min="11" max="11" width="42.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2047,9 +2071,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>18</v>
@@ -2073,18 +2097,22 @@
       <c r="I2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="17"/>
+      <c r="J2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="13" t="s">
@@ -2102,12 +2130,16 @@
       <c r="I3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="17"/>
+      <c r="J3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>18</v>
@@ -2129,14 +2161,18 @@
         <v>1</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="17"/>
+        <v>78</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>18</v>
@@ -2146,7 +2182,7 @@
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>21</v>
@@ -2160,12 +2196,16 @@
       <c r="I5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="17"/>
+      <c r="J5" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>18</v>
@@ -2175,7 +2215,7 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>6</v>
@@ -2189,12 +2229,16 @@
       <c r="I6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="17"/>
+      <c r="J6" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>18</v>
@@ -2204,10 +2248,10 @@
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>18</v>
@@ -2216,72 +2260,80 @@
         <v>1</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="12"/>
-      <c r="K7" s="17"/>
+        <v>28</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="17"/>
     </row>
-    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>18</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="17"/>
+        <v>35</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>18</v>
@@ -2291,7 +2343,7 @@
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="10" t="s">
@@ -2304,9 +2356,9 @@
       <c r="J10" s="12"/>
       <c r="K10" s="17"/>
     </row>
-    <row r="11" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>19</v>
@@ -2316,7 +2368,7 @@
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>10</v>
@@ -2328,14 +2380,14 @@
         <v>1</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="17"/>
     </row>
-    <row r="12" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>18</v>
@@ -2345,10 +2397,10 @@
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>18</v>
@@ -2358,31 +2410,31 @@
       </c>
       <c r="I12" s="16"/>
       <c r="J12" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>74</v>
-      </c>
       <c r="G13" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13" s="15">
         <v>3</v>
@@ -2391,25 +2443,25 @@
       <c r="J13" s="18"/>
       <c r="K13" s="17"/>
     </row>
-    <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>77</v>
-      </c>
       <c r="G14" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H14" s="15">
         <v>2</v>
@@ -2418,25 +2470,25 @@
       <c r="J14" s="18"/>
       <c r="K14" s="17"/>
     </row>
-    <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="G15" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>65</v>
       </c>
       <c r="H15" s="15">
         <v>1</v>
@@ -2445,25 +2497,25 @@
       <c r="J15" s="18"/>
       <c r="K15" s="17"/>
     </row>
-    <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>68</v>
-      </c>
       <c r="G16" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16" s="15">
         <v>1</v>
@@ -2472,25 +2524,25 @@
       <c r="J16" s="18"/>
       <c r="K16" s="17"/>
     </row>
-    <row r="17" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>71</v>
-      </c>
       <c r="G17" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" s="15">
         <v>1</v>
@@ -2499,19 +2551,19 @@
       <c r="J17" s="18"/>
       <c r="K17" s="17"/>
     </row>
-    <row r="18" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>9</v>
@@ -2520,29 +2572,29 @@
         <v>19</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
     </row>
-    <row r="19" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>9</v>
@@ -2551,27 +2603,27 @@
         <v>19</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
     </row>
-    <row r="20" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>9</v>
@@ -2580,17 +2632,17 @@
         <v>19</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
     </row>
-    <row r="21" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>19</v>
@@ -2600,7 +2652,7 @@
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>7</v>
@@ -2610,14 +2662,14 @@
         <v>1</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J21" s="12"/>
       <c r="K21" s="17"/>
     </row>
-    <row r="22" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>19</v>
@@ -2637,14 +2689,14 @@
         <v>1</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="17"/>
     </row>
-    <row r="23" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>19</v>
@@ -2654,7 +2706,7 @@
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>9</v>
@@ -2664,20 +2716,27 @@
         <v>1</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="17"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K4" r:id="rId1" xr:uid="{FDACA401-9263-4EBB-A0A1-4B6A09A1C0C7}"/>
+    <hyperlink ref="K2:K3" r:id="rId2" display="https://s.click.aliexpress.com/e/_Ao9yaZ" xr:uid="{4DE29B24-5FB8-4512-8258-A99500703709}"/>
+    <hyperlink ref="K5" r:id="rId3" xr:uid="{4DCC8F85-4E77-4A39-98FC-004EDAB005FB}"/>
+    <hyperlink ref="K6:K7" r:id="rId4" display="https://s.click.aliexpress.com/e/_Ao9yaZ" xr:uid="{07E9BAE6-A96E-4A15-A95E-FA50F52DC663}"/>
+    <hyperlink ref="K9" r:id="rId5" xr:uid="{472705C6-23F1-49F5-AB9D-302E44600814}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId6"/>
   <webPublishItems count="2">
     <webPublishItem id="16836" divId="BOM_HextrudORT_Extruder_NOVA_16836" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\HOTEND_EXTRUDER\NOVA\BOM_HextrudORT_Extruder_NOVA.htm" autoRepublish="1"/>
     <webPublishItem id="24158" divId="BOM_HextrudORT_Extruder_Dragon_24158" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\HOTEND_EXTRUDER\DRAGON\BOM_HextrudORT_Extruder_Dragon.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bondtech BMG part details
</commit_message>
<xml_diff>
--- a/files/HOTEND_EXTRUDER/DRAGON/BOM_HextrudORT_Extruder_Dragon.xlsx
+++ b/files/HOTEND_EXTRUDER/DRAGON/BOM_HextrudORT_Extruder_Dragon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\HOTEND_EXTRUDER\DRAGON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D312B1B-C356-4A76-AB0D-2BD8E0574AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9774A9D4-BD1C-42CF-8F32-AC1E0C39E51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="85">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -37,12 +37,6 @@
     <t>Vendor URL</t>
   </si>
   <si>
-    <t>Comes with BMG</t>
-  </si>
-  <si>
-    <t>Make From BMG arm pin</t>
-  </si>
-  <si>
     <t>3D_Printed</t>
   </si>
   <si>
@@ -55,9 +49,6 @@
     <t>Comes with BMG clones</t>
   </si>
   <si>
-    <t>SetScrew_M3X2_92605A097</t>
-  </si>
-  <si>
     <t>SubAssy</t>
   </si>
   <si>
@@ -82,18 +73,9 @@
     <t>MAKE</t>
   </si>
   <si>
-    <t>Bondetech mini gears v1</t>
-  </si>
-  <si>
-    <t>From BMG extruder</t>
-  </si>
-  <si>
     <t>From BMG Extruder</t>
   </si>
   <si>
-    <t>Bondtech_Shaft_assembly v1</t>
-  </si>
-  <si>
     <t>Bondtech_Thumbscrew_assembly v1</t>
   </si>
   <si>
@@ -103,75 +85,10 @@
     <t>PTFE Tube Retainer</t>
   </si>
   <si>
-    <t>Retainer, PTFE Tube 4mm</t>
-  </si>
-  <si>
-    <t>Is included with certain BMG clones.
-If not, need to purchase separately</t>
-  </si>
-  <si>
     <t>6a</t>
   </si>
   <si>
-    <t>OPTION A: Bearing_MR95_7804K105</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="3"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OPTION A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-These are BIGGER bearings than the ones used in the BMG.
- To be used with Back Plate and cover marked with "BB"</t>
-    </r>
-  </si>
-  <si>
     <t>6b</t>
-  </si>
-  <si>
-    <t>OPTION B: Bearing_MR85 (from BMG)</t>
-  </si>
-  <si>
-    <t>Bearing 5X8X2.5</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="3"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OPTION B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Use MR85 5x8x2.5 bearings from BMG</t>
-    </r>
   </si>
   <si>
     <t>PTFE_Guide</t>
@@ -181,9 +98,6 @@
 1 - Using Xacto blade, create internal chamfer in one end.
 2 - Cut that end into an arrow shape (try to match the angle from the HextrudORT body where the hobb gears meet.
 3 - Insert into HextrudORT body and cut excess length flush. </t>
-  </si>
-  <si>
-    <t>1a</t>
   </si>
   <si>
     <t>bltouch</t>
@@ -354,32 +268,113 @@
     <t>HARDWARE</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">From BMG Extruder
-</t>
-    </r>
+    <t>Bondtech BMG parts</t>
+  </si>
+  <si>
+    <t>Bondetech mini gears 1.75/5.0</t>
+  </si>
+  <si>
+    <t>From BMG extruder or sold seperately</t>
+  </si>
+  <si>
+    <t>Gear set for filament size 1.75 mm, primary gear with inner diameter 5 mm, secondary gear with two needle bearings,M3x2 setscrew and one 3 x 20 mm shaft.</t>
+  </si>
+  <si>
+    <t>Bondtech</t>
+  </si>
+  <si>
+    <t>https://www.bondtech.se/product/drivegear-kits/</t>
+  </si>
+  <si>
+    <t>Bondtech_Shaft_assembly</t>
+  </si>
+  <si>
+    <t>Replacement Shaft assembly for our Bondtech Mini Geared (BMG), SingleDirect and DualDirect extruders.
+It includes the set screw for primary 1.75/5.0 drive gear.</t>
+  </si>
+  <si>
+    <t>https://www.bondtech.se/product/shaft-assembly/</t>
+  </si>
+  <si>
+    <t>https://www.bondtech.se/product/thumbscrew-assembly/</t>
+  </si>
+  <si>
+    <t>Make From BMG arm pin
+3 X 20mm or sold seperately</t>
+  </si>
+  <si>
+    <t>From BMG Extruder 3 X 20</t>
+  </si>
+  <si>
+    <t>https://www.bondtech.se/product/shafts/</t>
+  </si>
+  <si>
+    <t>Retainer, PTFE Tube 4mm
+From BMG or sold seperately</t>
+  </si>
+  <si>
+    <t>https://www.bondtech.se/product/push-fit-collar/</t>
+  </si>
+  <si>
+    <t>OPTION A: Bearing_MR85 (from BMG)</t>
+  </si>
+  <si>
+    <t>Bearing 5X8X2.5 From BMG or sold seperately</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color theme="3"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>*NOTE*
-1 - Some BMG clone have a 4mm thick gear, they will not fit.
-  Verified sources are: 
-  a) Original BMG from BondTech
-  b) https://s.click.aliexpress.com/e/_Ao9yaZ
-2 -  Short side of the shaft might need to be filed down to avoid grinding against stepper motor.</t>
+      <t>OPTION A</t>
     </r>
-  </si>
-  <si>
-    <t>https://s.click.aliexpress.com/e/_Ao9yaZ</t>
-  </si>
-  <si>
-    <t>Triangle Lab</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Use MR85 5x8x2.5 bearings from BMG</t>
+    </r>
+  </si>
+  <si>
+    <t>OPTION B: Bearing_MR95_7804K105</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OPTION B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+These are BIGGER bearings than the ones used in the BMG.
+ To be used with Back Plate and cover marked with "BB"</t>
+    </r>
+  </si>
+  <si>
+    <t>Dragon HextrudORT</t>
   </si>
 </sst>
 </file>
@@ -489,14 +484,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -504,8 +491,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,6 +510,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD6EE22"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,9 +626,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -683,8 +684,29 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -753,13 +775,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>98425</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>155575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1235075</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>1292225</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -796,366 +818,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>536576</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>555626</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>946151</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>958851</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16" descr="thumbnail_16.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3635376" y="2416176"/>
-          <a:ext cx="409575" cy="403225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>193675</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1254125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17" descr="thumbnail_3.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C5264B3-4630-46F6-B569-81C76894859A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3032125" y="2044700"/>
-          <a:ext cx="1076325" cy="1069975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>193675</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1254125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18" descr="thumbnail_4.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32AB4877-2EEA-4A09-AEEC-0E15B2DD4D1C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3032125" y="603250"/>
-          <a:ext cx="1076325" cy="1069975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>193675</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1254125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19" descr="thumbnail_5.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57534616-CBDF-48E5-ACC9-755C14C4D902}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3032125" y="3486150"/>
-          <a:ext cx="1076325" cy="1069975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>193675</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1254125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21" descr="thumbnail_7.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8225F38D-7A74-4ECB-A83D-FCDAA1059355}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3032125" y="7810500"/>
-          <a:ext cx="1076325" cy="1069975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>193675</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1254125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22" descr="thumbnail_14.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CC656D1-1AC5-4268-8B1E-D52505D15013}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3032125" y="4927600"/>
-          <a:ext cx="1076325" cy="1069975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>193675</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1254125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 24" descr="thumbnail_19.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EC9C93C-0378-4CC2-9A5E-C67D0075A297}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3032125" y="6369050"/>
-          <a:ext cx="1076325" cy="1069975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>244475</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>215144</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1238250</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1203325</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Picture 26" descr="thumbnail_7.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0D8BF7F-9D79-46A6-B241-44169BA7AE2A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3082925" y="9286119"/>
-          <a:ext cx="993775" cy="985006"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1292225</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>1247775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1172,7 +842,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1193,13 +863,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>193675</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>1254125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1216,7 +886,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1237,13 +907,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1222375</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>1250950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1260,7 +930,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1281,13 +951,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>82550</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1184275</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>1247775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1304,7 +974,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1325,13 +995,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1292225</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>1257300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1348,7 +1018,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1369,13 +1039,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1292225</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>1263650</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1392,7 +1062,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1413,13 +1083,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1222375</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>1212850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1436,7 +1106,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1457,13 +1127,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>168275</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>1298575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1480,7 +1150,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1501,13 +1171,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>168275</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>1298575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1524,7 +1194,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1545,13 +1215,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>168275</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1298575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1568,7 +1238,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1589,13 +1259,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>168275</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>1298575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1612,7 +1282,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1633,13 +1303,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>168275</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>1298575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1656,7 +1326,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1673,12 +1343,320 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>193675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1266825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1254125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25" descr="thumbnail_4.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99C3DF73-8D9C-4E60-8271-A9F2F93AAE4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3406775" y="809625"/>
+          <a:ext cx="1073150" cy="1073150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>193675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1266825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1254125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29" descr="thumbnail_5.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D09BDB1-9F5B-4D18-BAA5-05BAD10BDC55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3406775" y="3679825"/>
+          <a:ext cx="1073150" cy="1073150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>193675</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1266825</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1254125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30" descr="thumbnail_7.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C37A60F-4B3B-4070-94F2-A74A386C4CDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3406775" y="9623425"/>
+          <a:ext cx="1073150" cy="1073150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>193675</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1266825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1254125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39" descr="thumbnail_14.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AFBFCB4-3837-49E1-94DA-AA08C40B8C6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3406775" y="5114925"/>
+          <a:ext cx="1073150" cy="1073150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>244475</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>215144</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1203325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40" descr="thumbnail_7.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3AFD3-8B97-41E8-96C2-A8414E0C029B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3457575" y="8019294"/>
+          <a:ext cx="993775" cy="988181"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1463675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1352813</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41" descr="thumbnail_1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4D22516-1213-4659-887E-656F43811794}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3390900" y="2190750"/>
+          <a:ext cx="1285875" cy="1225813"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>127001</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1352550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1327055</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42" descr="thumbnail_1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD5354D9-8E3D-48E7-9CBD-A020319DEB93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3340101" y="6527800"/>
+          <a:ext cx="1225549" cy="1168305"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{494CDCE7-8EB1-486A-8076-EC1E59242533}" name="Table1" displayName="Table1" ref="A1:K23" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
-  <autoFilter ref="A1:K23" xr:uid="{4DBD3307-5F20-47E0-9C75-3A8478E4F27D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{494CDCE7-8EB1-486A-8076-EC1E59242533}" name="Table1" displayName="Table1" ref="A1:K24" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+  <autoFilter ref="A1:K24" xr:uid="{4DBD3307-5F20-47E0-9C75-3A8478E4F27D}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{8DD10BD1-F8F8-4CF0-8D4C-7F4FC801B3C7}" name="SubAssy"/>
     <tableColumn id="2" xr3:uid="{48F8A639-6252-46BC-8E09-3A18B47C9DCC}" name="Category"/>
@@ -2017,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2038,13 +2016,13 @@
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -2053,16 +2031,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
@@ -2071,400 +2049,370 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="11">
-        <v>1</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="15">
-        <v>1</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>79</v>
-      </c>
+    <row r="2" spans="1:11" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>38</v>
+        <v>15</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="13" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H3" s="15">
         <v>1</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" s="11">
         <v>2</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="13" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H4" s="15">
         <v>1</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="11">
         <v>3</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H5" s="15">
         <v>1</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="11">
         <v>4</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H6" s="15">
         <v>1</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="11">
         <v>5</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H7" s="15">
         <v>1</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="17"/>
+        <v>81</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>79</v>
-      </c>
+    <row r="9" spans="1:11" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="11">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="14"/>
       <c r="G10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="15">
-        <v>1</v>
-      </c>
-      <c r="I10" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="J10" s="12"/>
       <c r="K10" s="17"/>
     </row>
-    <row r="11" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" s="11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>10</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F11" s="14"/>
       <c r="G11" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H11" s="15">
         <v>1</v>
       </c>
-      <c r="I11" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="I11" s="16"/>
       <c r="J11" s="12"/>
       <c r="K11" s="17"/>
     </row>
-    <row r="12" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="13" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H12" s="15">
         <v>1</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>59</v>
-      </c>
+      <c r="I12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="12"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>71</v>
+        <v>15</v>
+      </c>
+      <c r="C13" s="11">
+        <v>9</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="13" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="H13" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I13" s="16"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="17"/>
+      <c r="J13" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="13" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H14" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I14" s="16"/>
       <c r="J14" s="18"/>
@@ -2472,26 +2420,26 @@
     </row>
     <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>63</v>
-      </c>
       <c r="G15" s="10" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H15" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="18"/>
@@ -2499,23 +2447,23 @@
     </row>
     <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="13" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H16" s="15">
         <v>1</v>
@@ -2526,23 +2474,23 @@
     </row>
     <row r="17" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="13" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H17" s="15">
         <v>1</v>
@@ -2553,190 +2501,213 @@
     </row>
     <row r="18" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="16" t="s">
         <v>50</v>
       </c>
+      <c r="H18" s="15">
+        <v>1</v>
+      </c>
+      <c r="I18" s="16"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
     </row>
     <row r="19" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>46</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="13" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
     </row>
     <row r="20" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="12"/>
+        <v>27</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="E20" s="13" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="11">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="13" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="15">
-        <v>1</v>
+      <c r="G21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="J21" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="J21" s="18"/>
       <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C22" s="11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="13" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="15">
         <v>1</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="17"/>
     </row>
     <row r="23" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C23" s="11">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="13" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="15">
         <v>1</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="17"/>
     </row>
+    <row r="24" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="11">
+        <v>13</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" s="15">
+        <v>1</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="12"/>
+      <c r="K24" s="17"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K4" r:id="rId1" xr:uid="{FDACA401-9263-4EBB-A0A1-4B6A09A1C0C7}"/>
-    <hyperlink ref="K2:K3" r:id="rId2" display="https://s.click.aliexpress.com/e/_Ao9yaZ" xr:uid="{4DE29B24-5FB8-4512-8258-A99500703709}"/>
-    <hyperlink ref="K5" r:id="rId3" xr:uid="{4DCC8F85-4E77-4A39-98FC-004EDAB005FB}"/>
-    <hyperlink ref="K6:K7" r:id="rId4" display="https://s.click.aliexpress.com/e/_Ao9yaZ" xr:uid="{07E9BAE6-A96E-4A15-A95E-FA50F52DC663}"/>
-    <hyperlink ref="K9" r:id="rId5" xr:uid="{472705C6-23F1-49F5-AB9D-302E44600814}"/>
+    <hyperlink ref="K4" r:id="rId1" xr:uid="{36A725FB-217B-4926-A4C6-9CD024CCF556}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId2"/>
   <webPublishItems count="2">
     <webPublishItem id="16836" divId="BOM_HextrudORT_Extruder_NOVA_16836" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\HOTEND_EXTRUDER\NOVA\BOM_HextrudORT_Extruder_NOVA.htm" autoRepublish="1"/>
     <webPublishItem id="24158" divId="BOM_HextrudORT_Extruder_Dragon_24158" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\HOTEND_EXTRUDER\DRAGON\BOM_HextrudORT_Extruder_Dragon.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bondtech Kit reference added
</commit_message>
<xml_diff>
--- a/files/HOTEND_EXTRUDER/DRAGON/BOM_HextrudORT_Extruder_Dragon.xlsx
+++ b/files/HOTEND_EXTRUDER/DRAGON/BOM_HextrudORT_Extruder_Dragon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HextrudORT\files\HOTEND_EXTRUDER\DRAGON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F4AC54-B6E1-446F-A343-56A0DEF37EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC667C80-EFBC-4ED7-BEA8-AA72BE0777E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="80">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -274,16 +274,10 @@
     <t>Bondetech mini gears 1.75/5.0</t>
   </si>
   <si>
-    <t>From BMG extruder or sold seperately</t>
-  </si>
-  <si>
     <t>Gear set for filament size 1.75 mm, primary gear with inner diameter 5 mm, secondary gear with two needle bearings,M3x2 setscrew and one 3 x 20 mm shaft.</t>
   </si>
   <si>
     <t>Bondtech</t>
-  </si>
-  <si>
-    <t>https://www.bondtech.se/product/drivegear-kits/</t>
   </si>
   <si>
     <t>Bondtech_Shaft_assembly</t>
@@ -293,33 +287,10 @@
 It includes the set screw for primary 1.75/5.0 drive gear.</t>
   </si>
   <si>
-    <t>https://www.bondtech.se/product/shaft-assembly/</t>
-  </si>
-  <si>
-    <t>https://www.bondtech.se/product/thumbscrew-assembly/</t>
-  </si>
-  <si>
-    <t>Make From BMG arm pin
-3 X 20mm or sold seperately</t>
-  </si>
-  <si>
     <t>From BMG Extruder 3 X 20</t>
   </si>
   <si>
-    <t>https://www.bondtech.se/product/shafts/</t>
-  </si>
-  <si>
-    <t>Retainer, PTFE Tube 4mm
-From BMG or sold seperately</t>
-  </si>
-  <si>
-    <t>https://www.bondtech.se/product/push-fit-collar/</t>
-  </si>
-  <si>
     <t>OPTION A: Bearing_MR85 (from BMG)</t>
-  </si>
-  <si>
-    <t>Bearing 5X8X2.5 From BMG or sold seperately</t>
   </si>
   <si>
     <t>OPTION B: Bearing_MR95_7804K105</t>
@@ -378,7 +349,16 @@
     </r>
   </si>
   <si>
-    <t>https://www.bondtech.se/product/ballbearing-5x8x2-5/</t>
+    <t>Included in BMG Internals Set for HextrudORT</t>
+  </si>
+  <si>
+    <t>(BUY) KIT</t>
+  </si>
+  <si>
+    <t>https://www.bondtech.se/product/bmg-internals-set-for-hextrudort/</t>
+  </si>
+  <si>
+    <t>2*</t>
   </si>
 </sst>
 </file>
@@ -2002,7 +1982,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2083,22 +2063,22 @@
         <v>65</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="H3" s="15">
         <v>1</v>
       </c>
       <c r="I3" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="K3" s="19" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2113,25 +2093,25 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="H4" s="15">
         <v>1</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2149,10 +2129,10 @@
         <v>18</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="H5" s="15">
         <v>1</v>
@@ -2161,10 +2141,10 @@
         <v>17</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2182,22 +2162,22 @@
         <v>19</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="H6" s="15">
         <v>1</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2215,10 +2195,10 @@
         <v>20</v>
       </c>
       <c r="F7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="H7" s="15">
         <v>1</v>
@@ -2227,7 +2207,7 @@
         <v>17</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K7" s="19" t="s">
         <v>78</v>
@@ -2245,30 +2225,30 @@
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>33</v>
-      </c>
       <c r="I8" s="16" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -2293,7 +2273,7 @@
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="13" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>39</v>
@@ -2305,7 +2285,7 @@
         <v>33</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="17"/>
@@ -2702,12 +2682,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K4" r:id="rId1" xr:uid="{C0DAE444-8140-4D26-9D95-8DAB6D62E101}"/>
-    <hyperlink ref="K3" r:id="rId2" xr:uid="{C5584D40-61BB-40DC-9DE8-95A34106DC17}"/>
-    <hyperlink ref="K5" r:id="rId3" xr:uid="{E1B8DB0A-1739-43E9-87FE-7DA3E6AC4F67}"/>
-    <hyperlink ref="K6" r:id="rId4" xr:uid="{5BDB69E3-82F5-4D54-9175-F3B290A079F1}"/>
-    <hyperlink ref="K7" r:id="rId5" xr:uid="{C9AB9826-3752-479E-84B9-B2B671117D7C}"/>
-    <hyperlink ref="K8" r:id="rId6" xr:uid="{8602A601-D3B0-4077-819C-B325A82E0B49}"/>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{48E6D9EF-D3CC-4632-AF5B-F066AE980C97}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{ED13E1FE-81C8-412D-BCE7-9AF106557271}"/>
+    <hyperlink ref="K5" r:id="rId3" xr:uid="{CAF9E168-FC23-445B-9FA6-E6979B427F40}"/>
+    <hyperlink ref="K6" r:id="rId4" xr:uid="{8F4CD821-6110-4B00-A460-2F927C1CE339}"/>
+    <hyperlink ref="K7" r:id="rId5" xr:uid="{588B0F7E-8719-49E2-AB93-14267261991F}"/>
+    <hyperlink ref="K8" r:id="rId6" xr:uid="{ECF27C49-C14C-41EE-8C29-628DBB055F93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId7"/>

</xml_diff>